<commit_message>
cambiar un numéro de switch y configuración routers
Se configuro departamentos Youtube y Business, además del router del país EEUU
</commit_message>
<xml_diff>
--- a/Google_Distribuciones_Proyecto.xlsx
+++ b/Google_Distribuciones_Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilme\Desktop\Proyecto Redes\Proyecto_Redes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620D40F0-ECC4-4C66-94B5-26931E8C6AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBE45C7-607E-45A5-8965-05AAAFA9965B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{D019C2EC-662E-4189-B3CB-7C90BCE75419}"/>
+    <workbookView xWindow="2208" yWindow="1620" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{D019C2EC-662E-4189-B3CB-7C90BCE75419}"/>
   </bookViews>
   <sheets>
     <sheet name="Paises" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +646,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -659,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -718,6 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,14 +1111,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="17" max="17" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C2" s="10" t="s">
         <v>96</v>
       </c>
@@ -1122,7 +1129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>300</v>
       </c>
@@ -1140,7 +1147,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>300</v>
       </c>
@@ -1158,7 +1165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>350</v>
       </c>
@@ -1176,7 +1183,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>350</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>400</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8">
         <f>SUM(C3:C7)</f>
         <v>2000</v>
@@ -1232,24 +1239,24 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1269,7 +1276,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>52</v>
       </c>
@@ -1280,7 +1287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>13</v>
       </c>
@@ -1311,7 +1318,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1325,7 +1332,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1339,7 +1346,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1358,7 +1365,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1380,7 +1387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1388,7 +1395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -1399,7 +1406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
@@ -1415,7 +1422,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1437,21 +1444,21 @@
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1"/>
-    <col min="12" max="12" width="3.5703125" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" customWidth="1"/>
+    <col min="12" max="12" width="3.5546875" customWidth="1"/>
+    <col min="14" max="14" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:15" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A1" s="14" t="s">
         <v>97</v>
       </c>
@@ -1462,7 +1469,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="N2" s="17" t="s">
         <v>26</v>
       </c>
@@ -1470,7 +1477,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>52</v>
       </c>
@@ -1525,7 +1532,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -1558,7 +1565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -1587,7 +1594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1622,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1648,7 +1655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1678,7 +1685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1698,7 +1705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1731,7 +1738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1751,7 +1758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <f>SUM(B3,B5,B7,B11,)</f>
@@ -1800,7 +1807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="N15" s="17" t="s">
         <v>14</v>
       </c>
@@ -1808,7 +1815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <f>SUM(B14:J14)</f>
         <v>370</v>
@@ -1820,7 +1827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="N17" t="s">
         <v>25</v>
       </c>
@@ -1828,7 +1835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1843,7 +1850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>A3:B3</f>
         <v>Acces</v>
@@ -1881,7 +1888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>A5</f>
         <v>GoggleCloud</v>
@@ -1917,7 +1924,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>A7</f>
         <v>Youtube</v>
@@ -1949,7 +1956,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>A11</f>
         <v>Marketing</v>
@@ -1980,7 +1987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>C3</f>
         <v>Waymo</v>
@@ -1998,7 +2005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>C5</f>
         <v>Bussiness</v>
@@ -2016,7 +2023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>C9</f>
         <v>StrategicPartnerships</v>
@@ -2034,7 +2041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -2042,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -2050,7 +2057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -2061,13 +2068,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B30">
         <f>B29*C29</f>
         <v>408</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B31">
         <f>SUM(B27:B30)</f>
         <v>435</v>
@@ -2076,7 +2083,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B32">
         <f>B31-C31</f>
         <v>26</v>
@@ -2093,22 +2100,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA27DE7-FAAC-4D5D-A440-617AB89B6881}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>105</v>
       </c>
@@ -2128,7 +2135,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>26</v>
       </c>
@@ -2150,8 +2157,13 @@
       <c r="H2" s="18" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
@@ -2165,7 +2177,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -2173,8 +2185,13 @@
       <c r="H3" s="18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>41</v>
       </c>
@@ -2194,8 +2211,13 @@
       <c r="H4" s="18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>51</v>
       </c>
@@ -2218,7 +2240,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
@@ -2239,7 +2261,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
@@ -2260,7 +2282,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -2283,7 +2305,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>104</v>
       </c>
@@ -2306,7 +2328,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
@@ -2327,7 +2349,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
@@ -2349,7 +2371,7 @@
       </c>
       <c r="K11" s="25"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>39</v>
       </c>
@@ -2372,7 +2394,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>16</v>
       </c>
@@ -2393,7 +2415,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
@@ -2416,7 +2438,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>14</v>
       </c>
@@ -2431,7 +2453,7 @@
       </c>
       <c r="E15" s="29"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
@@ -2448,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
@@ -2463,7 +2485,7 @@
       </c>
       <c r="E17" s="28"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
@@ -2478,7 +2500,7 @@
       </c>
       <c r="E18" s="28"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>35</v>
       </c>
@@ -2493,13 +2515,13 @@
       </c>
       <c r="E19" s="28"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C22" s="19"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E24" s="22"/>
     </row>
   </sheetData>
@@ -2524,24 +2546,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAB763C-F027-4071-A3AD-C2AEA1EF48DC}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +2571,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2557,7 +2579,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2565,7 +2587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2588,7 +2610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2596,7 +2618,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -2604,7 +2626,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>66</v>
       </c>
@@ -2612,7 +2634,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
@@ -2626,7 +2648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -2643,7 +2665,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -2660,7 +2682,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>64</v>
       </c>
@@ -2677,7 +2699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -2694,7 +2716,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>85</v>
       </c>

</xml_diff>